<commit_message>
finish admin side dash bord
</commit_message>
<xml_diff>
--- a/path_to_your_file.xlsx
+++ b/path_to_your_file.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="63">
   <si>
     <t>Order No</t>
   </si>
@@ -133,16 +133,73 @@
     <t>$958</t>
   </si>
   <si>
+    <t>2024-05-27</t>
+  </si>
+  <si>
+    <t>wildcraft</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>$150</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> laptop bag2, Hp laptop bag</t>
+  </si>
+  <si>
+    <t>3, 5</t>
+  </si>
+  <si>
+    <t>%, 20</t>
+  </si>
+  <si>
+    <t>144$, 80</t>
+  </si>
+  <si>
+    <t>$807</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> laptop bag3</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>$950</t>
+  </si>
+  <si>
+    <t>2024-05-30</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Total Orders: 5</t>
-  </si>
-  <si>
-    <t>TotalDiscount: $362</t>
-  </si>
-  <si>
-    <t>Total Sales: $2902</t>
+    <t>250</t>
+  </si>
+  <si>
+    <t>$1250</t>
+  </si>
+  <si>
+    <t>Total Orders: 9</t>
+  </si>
+  <si>
+    <t>TotalDiscount: $175</t>
+  </si>
+  <si>
+    <t>Total Sales: $6059</t>
   </si>
 </sst>
 </file>
@@ -519,7 +576,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J12"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
@@ -612,6 +669,9 @@
       <c r="F3" t="s">
         <v>21</v>
       </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
       <c r="H3" t="s">
         <v>22</v>
       </c>
@@ -641,6 +701,9 @@
       <c r="F4" t="s">
         <v>26</v>
       </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
       <c r="H4" t="s">
         <v>27</v>
       </c>
@@ -715,30 +778,152 @@
         <v>17</v>
       </c>
     </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>513307</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" t="s">
+        <v>45</v>
+      </c>
+      <c r="I7" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" t="s">
+        <v>17</v>
+      </c>
+    </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>40</v>
+      <c r="A8">
+        <v>474100</v>
       </c>
       <c r="B8" t="s">
         <v>40</v>
       </c>
       <c r="C8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" t="s">
+        <v>49</v>
+      </c>
+      <c r="G8">
+        <v>25</v>
+      </c>
+      <c r="H8" t="s">
+        <v>50</v>
+      </c>
+      <c r="I8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>639057</v>
+      </c>
+      <c r="B9" t="s">
         <v>40</v>
       </c>
-      <c r="D8" t="s">
+      <c r="C9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9">
+        <v>50</v>
+      </c>
+      <c r="H9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I9" t="s">
+        <v>16</v>
+      </c>
+      <c r="J9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>916703</v>
+      </c>
+      <c r="B10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" t="s">
         <v>41</v>
       </c>
-      <c r="G8" t="s">
-        <v>42</v>
-      </c>
-      <c r="H8" t="s">
-        <v>43</v>
-      </c>
-      <c r="I8" t="s">
-        <v>40</v>
-      </c>
-      <c r="J8" t="s">
-        <v>40</v>
+      <c r="D10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" t="s">
+        <v>58</v>
+      </c>
+      <c r="H10" t="s">
+        <v>59</v>
+      </c>
+      <c r="I10" t="s">
+        <v>28</v>
+      </c>
+      <c r="J10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12" t="s">
+        <v>61</v>
+      </c>
+      <c r="H12" t="s">
+        <v>62</v>
+      </c>
+      <c r="I12" t="s">
+        <v>57</v>
+      </c>
+      <c r="J12" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>